<commit_message>
Edited GUITestCases XLS file to edit one test sheet
</commit_message>
<xml_diff>
--- a/website_tests/kdf/data/GUITestCases.xlsx
+++ b/website_tests/kdf/data/GUITestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manmeetchadha/seleniumprojects/elevatederm/website_tests/kdf/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manmeetchadha/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432FD2AF-B4E8-7E4A-9658-67E91295AFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BECECC7-C055-0A47-A3F5-6CA44420CD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8940" yWindow="1020" windowWidth="28280" windowHeight="18640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6033" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6053" uniqueCount="840">
   <si>
     <t>TESTCASE_ID</t>
   </si>
@@ -2554,6 +2554,21 @@
   </si>
   <si>
     <t>Verify text on page after the login action is complete</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>react-burger-menu-btn</t>
+  </si>
+  <si>
+    <t>logout_sidebar_link</t>
+  </si>
+  <si>
+    <t>Click the main menu item</t>
+  </si>
+  <si>
+    <t>Click the required link</t>
   </si>
 </sst>
 </file>
@@ -15671,10 +15686,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15884,105 +15899,101 @@
       <c r="G9" s="39"/>
     </row>
     <row r="10" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="A10" s="36" t="s">
+        <v>815</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>836</v>
+      </c>
       <c r="F10" s="42"/>
       <c r="G10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="40"/>
+      <c r="A11" s="36" t="s">
+        <v>815</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>839</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>837</v>
+      </c>
+      <c r="F11" s="42"/>
       <c r="G11" s="39"/>
     </row>
-    <row r="12" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
-        <v>827</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>816</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="G12" s="39" t="s">
-        <v>820</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
-        <v>827</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>830</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>282</v>
-      </c>
+    <row r="12" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
-      <c r="F13" s="38" t="s">
-        <v>283</v>
-      </c>
+      <c r="F13" s="40"/>
       <c r="G13" s="39"/>
-      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>827</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>831</v>
+        <v>115</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>27</v>
+        <v>816</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>817</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>820</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="15" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>827</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>817</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="38" t="s">
-        <v>823</v>
+        <v>283</v>
       </c>
       <c r="G15" s="39"/>
       <c r="H15" s="5"/>
@@ -16001,7 +16012,7 @@
         <v>145</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F16" s="38"/>
       <c r="G16" s="39"/>
@@ -16021,20 +16032,20 @@
         <v>145</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>824</v>
+        <v>835</v>
       </c>
       <c r="G17" s="39"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>827</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C18" s="38" t="s">
         <v>27</v>
@@ -16043,38 +16054,118 @@
         <v>145</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>819</v>
-      </c>
-      <c r="F18" s="40"/>
+        <v>818</v>
+      </c>
+      <c r="F18" s="38"/>
       <c r="G18" s="39"/>
-    </row>
-    <row r="19" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>827</v>
       </c>
       <c r="B19" s="37" t="s">
+        <v>832</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>818</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="G19" s="39"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
+        <v>827</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>833</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>819</v>
+      </c>
+      <c r="F20" s="40"/>
+      <c r="G20" s="39"/>
+    </row>
+    <row r="21" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
+        <v>827</v>
+      </c>
+      <c r="B21" s="37" t="s">
         <v>834</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C21" s="38" t="s">
         <v>528</v>
       </c>
-      <c r="D19" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="38" t="s">
+      <c r="D21" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="38" t="s">
         <v>828</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F21" s="40" t="s">
         <v>829</v>
       </c>
-      <c r="G19" s="39"/>
+      <c r="G21" s="39"/>
+    </row>
+    <row r="22" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
+        <v>827</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="F22" s="42"/>
+      <c r="G22" s="39"/>
+    </row>
+    <row r="23" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="36" t="s">
+        <v>827</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>839</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>837</v>
+      </c>
+      <c r="F23" s="42"/>
+      <c r="G23" s="39"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="http://test.qurasense.com" xr:uid="{F9633516-7C7E-024A-B3C0-F7E5B704D642}"/>
     <hyperlink ref="F2" r:id="rId2" display="http://test.qurasense.com" xr:uid="{5071F030-5F69-FE42-B546-EADFEAEAE502}"/>
-    <hyperlink ref="G12" r:id="rId3" display="http://test.qurasense.com" xr:uid="{46B00015-AC01-7146-A4CB-EEE70006233C}"/>
-    <hyperlink ref="F12" r:id="rId4" display="http://test.qurasense.com" xr:uid="{81B30036-F71A-E044-9EA0-DC7372F4EF07}"/>
+    <hyperlink ref="G14" r:id="rId3" display="http://test.qurasense.com" xr:uid="{46B00015-AC01-7146-A4CB-EEE70006233C}"/>
+    <hyperlink ref="F14" r:id="rId4" display="http://test.qurasense.com" xr:uid="{81B30036-F71A-E044-9EA0-DC7372F4EF07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created a separate robot file for API calls.
</commit_message>
<xml_diff>
--- a/website_tests/kdf/data/GUITestCases.xlsx
+++ b/website_tests/kdf/data/GUITestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manmeetchadha/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manmeetchadha/seleniumtestautomation/website_tests/kdf/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BECECC7-C055-0A47-A3F5-6CA44420CD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F242A371-9ABD-7A43-A119-6E3945B8F8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="1020" windowWidth="28280" windowHeight="18640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="1020" windowWidth="28280" windowHeight="18640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuites" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6053" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6043" uniqueCount="840">
   <si>
     <t>TESTCASE_ID</t>
   </si>
@@ -15686,10 +15686,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16121,44 +16121,6 @@
         <v>829</v>
       </c>
       <c r="G21" s="39"/>
-    </row>
-    <row r="22" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
-        <v>827</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>838</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>836</v>
-      </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="39"/>
-    </row>
-    <row r="23" spans="1:8" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36" t="s">
-        <v>827</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>839</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>837</v>
-      </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="39"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>